<commit_message>
Disable format guessing (#15)
</commit_message>
<xml_diff>
--- a/src/ExcelsiorSyncfusion.Tests/DateFormats.Test.verified.xlsx
+++ b/src/ExcelsiorSyncfusion.Tests/DateFormats.Test.verified.xlsx
@@ -89,7 +89,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
@@ -117,6 +117,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -167,7 +170,7 @@
       <c r="B2" s="2">
         <v>44105.270833333336</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>